<commit_message>
update element id number for rules 0013 and 0014
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0014/DQC_0014_ListOfElements_V2.xlsx
+++ b/docs/DQC_US_0014/DQC_0014_ListOfElements_V2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26230"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellpryde/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanyount/Documents/dqc_us_rules/docs/DQC_US_0014/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="5840" windowWidth="36160" windowHeight="21640" tabRatio="500"/>
+    <workbookView xWindow="19080" yWindow="3520" windowWidth="36160" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -285,7 +285,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -299,11 +299,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -321,8 +316,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14.4"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,12 +338,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -353,34 +353,33 @@
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -668,17 +667,19 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.83203125" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="5"/>
-    <col min="9" max="9" width="150" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="71.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="10"/>
+    <col min="9" max="9" width="150" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -703,703 +704,703 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2774</v>
-      </c>
-      <c r="E2" s="4" t="s">
+    <row r="2" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2786</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2775</v>
-      </c>
-      <c r="E3" s="4" t="s">
+    <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2787</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2776</v>
-      </c>
-      <c r="E4" s="4" t="s">
+    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2788</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7">
-        <v>2777</v>
-      </c>
-      <c r="E5" s="4" t="s">
+    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2789</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2778</v>
-      </c>
-      <c r="E6" s="4" t="s">
+    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2790</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2779</v>
-      </c>
-      <c r="E7" s="4" t="s">
+    <row r="7" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2791</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2780</v>
-      </c>
-      <c r="E8" s="4" t="s">
+    <row r="8" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2792</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="7">
-        <v>2781</v>
-      </c>
-      <c r="E9" s="4" t="s">
+    <row r="9" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2793</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2782</v>
-      </c>
-      <c r="E10" s="4" t="s">
+    <row r="10" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2794</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7">
-        <v>2783</v>
-      </c>
-      <c r="E11" s="4" t="s">
+    <row r="11" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2795</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2784</v>
-      </c>
-      <c r="E12" s="4" t="s">
+    <row r="12" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2796</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="F12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2785</v>
-      </c>
-      <c r="E13" s="4" t="s">
+    <row r="13" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2797</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2786</v>
-      </c>
-      <c r="E14" s="4" t="s">
+    <row r="14" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2798</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="7">
-        <v>2787</v>
-      </c>
-      <c r="E15" s="4" t="s">
+    <row r="15" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2799</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="F15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2">
-        <v>2788</v>
-      </c>
-      <c r="E16" s="4" t="s">
+    <row r="16" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2800</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="F16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="7">
-        <v>2789</v>
-      </c>
-      <c r="E17" s="4" t="s">
+    <row r="17" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2801</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="F17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2">
-        <v>2790</v>
-      </c>
-      <c r="E18" s="4" t="s">
+    <row r="18" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2802</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="F18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="7">
-        <v>2791</v>
-      </c>
-      <c r="E19" s="4" t="s">
+    <row r="19" spans="1:9" ht="49" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2803</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="F19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2">
-        <v>2792</v>
-      </c>
-      <c r="E20" s="4" t="s">
+    <row r="20" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2804</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="F20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="7">
-        <v>2793</v>
-      </c>
-      <c r="E21" s="4" t="s">
+    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2805</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="F21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="2">
-        <v>2794</v>
-      </c>
-      <c r="E22" s="4" t="s">
+    <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2806</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="F22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="7">
-        <v>2795</v>
-      </c>
-      <c r="E23" s="4" t="s">
+    <row r="23" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2807</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="F23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="2">
-        <v>2796</v>
-      </c>
-      <c r="E24" s="4" t="s">
+    <row r="24" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2808</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="3" t="s">
+      <c r="F24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="7">
-        <v>2797</v>
-      </c>
-      <c r="E25" s="4" t="s">
+    <row r="25" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2809</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="3" t="s">
+      <c r="F25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I25" s="8" t="s">
@@ -1407,15 +1408,15 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>